<commit_message>
Opening for all activities
</commit_message>
<xml_diff>
--- a/Teams/MIndful.xlsx
+++ b/Teams/MIndful.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maryannleslie/Documents/Study/cse210/Teams/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2CBA68F-AEDE-8C48-955F-3733AF79DECE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{842AD617-6172-3A44-B659-3800920843DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2460" yWindow="500" windowWidth="24360" windowHeight="16220" xr2:uid="{4A463EAE-0E64-B443-851D-D1933B0E7F97}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Menu</t>
   </si>
@@ -116,6 +116,12 @@
   </si>
   <si>
     <t>3. Activity is never explicitly callen, only as a base for the subclasses.</t>
+  </si>
+  <si>
+    <t>DisplayStartMessage(): string</t>
+  </si>
+  <si>
+    <t>DisplayEndMessage(): string</t>
   </si>
 </sst>
 </file>
@@ -486,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3647C66-2434-AE4E-A837-32670EA727C2}">
-  <dimension ref="A2:G23"/>
+  <dimension ref="A2:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -498,13 +504,13 @@
     <col min="2" max="2" width="5.6640625" style="1" customWidth="1"/>
     <col min="3" max="3" width="29.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="5.5" style="1" customWidth="1"/>
-    <col min="5" max="5" width="26.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="29.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="5.33203125" style="1" customWidth="1"/>
     <col min="7" max="7" width="23.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -512,7 +518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>22</v>
       </c>
@@ -520,22 +526,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -543,89 +549,99 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E8" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E9" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E11" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E12" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="E13" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="2" t="s">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="1" t="s">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G18" s="1" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="G18" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G21" s="1" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
         <v>26</v>
       </c>
     </row>

</xml_diff>